<commit_message>
Removed React components, converted latter into sql files to analyse using SQL and Python (schema and data_import), updated development notes
</commit_message>
<xml_diff>
--- a/data-practice/processed/Compounded Shipping Container Data (PROCESSED).xlsx
+++ b/data-practice/processed/Compounded Shipping Container Data (PROCESSED).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Banette\Documents\Container Housing Feasibility\data-practice\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D4E6FF-B737-4814-934C-BC6E3E4520AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B4F7E4-3AFC-4F69-8596-3BB492410479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{6DCA420D-D163-4EC7-B169-BE2699A9998C}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23040" windowHeight="12120" activeTab="6" xr2:uid="{6DCA420D-D163-4EC7-B169-BE2699A9998C}"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="4" r:id="rId1"/>
@@ -1604,39 +1604,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="88">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1868,6 +1835,39 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1885,19 +1885,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F94B6A3A-2FBE-4779-995B-09C203B94792}" name="container_shipping_2017_complete" displayName="container_shipping_2017_complete" ref="A1:M27" totalsRowShown="0">
   <autoFilter ref="A1:M27" xr:uid="{F94B6A3A-2FBE-4779-995B-09C203B94792}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C3CC639D-A44D-4E34-BAFD-804B7154B4BB}" name="container_id" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A7A5FBBC-1452-45E6-BD39-2DBD8A461610}" name="ship_date" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{B9B0B228-3BEB-4790-9D90-7F90728B6733}" name="delivery_date" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A27B466F-3EB8-49E9-90C0-ACE9C2DE6C49}" name="producer" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{853C922E-AF69-4992-9872-0B5A118561F6}" name="producer_type" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{FA37F4BA-A16D-4FEA-811C-1694F6FDBFAA}" name="container_type" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{78ACA84E-CFDD-4628-9797-1A2D32982A08}" name="container_qty" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{EA4361A4-52CD-4C54-8696-B64158F1B600}" name="origin" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{96BAF35C-8DE0-42DA-B7BF-B62293E3C9FF}" name="destination" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{C3CC639D-A44D-4E34-BAFD-804B7154B4BB}" name="container_id" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{A7A5FBBC-1452-45E6-BD39-2DBD8A461610}" name="ship_date" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{B9B0B228-3BEB-4790-9D90-7F90728B6733}" name="delivery_date" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{A27B466F-3EB8-49E9-90C0-ACE9C2DE6C49}" name="producer" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{853C922E-AF69-4992-9872-0B5A118561F6}" name="producer_type" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{FA37F4BA-A16D-4FEA-811C-1694F6FDBFAA}" name="container_type" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{78ACA84E-CFDD-4628-9797-1A2D32982A08}" name="container_qty" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{EA4361A4-52CD-4C54-8696-B64158F1B600}" name="origin" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{96BAF35C-8DE0-42DA-B7BF-B62293E3C9FF}" name="destination" dataDxfId="79"/>
     <tableColumn id="10" xr3:uid="{1B12DCF8-2E84-442D-AB0C-552B01E24A22}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{07B3083D-935D-4E23-8289-16EE63CACA8A}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{C3288AF6-670E-433F-8B81-3773BDF7969D}" name="priority" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{EF2931C6-A503-421A-A994-D0EE174C89A3}" name="status" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{C3288AF6-670E-433F-8B81-3773BDF7969D}" name="priority" dataDxfId="78"/>
+    <tableColumn id="13" xr3:uid="{EF2931C6-A503-421A-A994-D0EE174C89A3}" name="status" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1907,19 +1907,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1182D5F8-ED85-4BC8-9F3F-EAA5312A76AA}" name="_2018" displayName="_2018" ref="A1:M31" totalsRowShown="0">
   <autoFilter ref="A1:M31" xr:uid="{1182D5F8-ED85-4BC8-9F3F-EAA5312A76AA}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E68853FC-288D-4679-A1DE-760AE41DC318}" name="container_id" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{74CBE9BB-B3D5-4771-A6C0-21992837B009}" name="ship_date" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{C5C64249-F10D-46E5-833B-866672B976B9}" name="delivery_date" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{61D60673-5784-419A-8F09-95B041C8BF68}" name="producer" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{8E3380A7-A82D-41FF-A71C-FE0B8D513F89}" name="producer_type" dataDxfId="83"/>
-    <tableColumn id="6" xr3:uid="{F7ED6D56-1C5A-4D3C-974F-EB06CC506E8F}" name="container_type" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{179ACF01-A242-4558-A3FA-8459E5AD044A}" name="container_qty" dataDxfId="81"/>
-    <tableColumn id="8" xr3:uid="{9B394FB2-E567-4EAD-BA24-220C71642B95}" name="origin" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{32A561F1-665F-4C8C-9C3C-EEB663CE71D9}" name="destination" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{E68853FC-288D-4679-A1DE-760AE41DC318}" name="container_id" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{74CBE9BB-B3D5-4771-A6C0-21992837B009}" name="ship_date" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{C5C64249-F10D-46E5-833B-866672B976B9}" name="delivery_date" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{61D60673-5784-419A-8F09-95B041C8BF68}" name="producer" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{8E3380A7-A82D-41FF-A71C-FE0B8D513F89}" name="producer_type" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{F7ED6D56-1C5A-4D3C-974F-EB06CC506E8F}" name="container_type" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{179ACF01-A242-4558-A3FA-8459E5AD044A}" name="container_qty" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{9B394FB2-E567-4EAD-BA24-220C71642B95}" name="origin" dataDxfId="69"/>
+    <tableColumn id="9" xr3:uid="{32A561F1-665F-4C8C-9C3C-EEB663CE71D9}" name="destination" dataDxfId="68"/>
     <tableColumn id="10" xr3:uid="{498EDBAB-8B36-4589-BF39-B7D9B81E59C1}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{9A6356E0-4E0A-4956-AA7B-4B2E268FD80C}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{C92F2241-B88F-4C50-92FE-048543650DE6}" name="priority" dataDxfId="78"/>
-    <tableColumn id="13" xr3:uid="{283260D9-54E0-4BB1-A8D4-6A4BC1E1AA92}" name="status" dataDxfId="77"/>
+    <tableColumn id="12" xr3:uid="{C92F2241-B88F-4C50-92FE-048543650DE6}" name="priority" dataDxfId="67"/>
+    <tableColumn id="13" xr3:uid="{283260D9-54E0-4BB1-A8D4-6A4BC1E1AA92}" name="status" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1929,19 +1929,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A7EFA01F-2EBB-4158-A397-16AF63979B1B}" name="_2019" displayName="_2019" ref="A1:M26" totalsRowShown="0">
   <autoFilter ref="A1:M26" xr:uid="{A7EFA01F-2EBB-4158-A397-16AF63979B1B}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{920927B9-F1FA-4827-887D-A0E268BEBD96}" name="container_id" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{2EC2CAEA-FB3C-4A4C-A288-E3E88A9D2E10}" name="ship_date" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{4434C7DA-1267-4C06-8242-3DE437A4BEDF}" name="delivery_date" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{D4311A9E-E2B3-4ED9-A989-6060DB766272}" name="producer" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{3EC2CE9B-5192-4531-A823-B61192F2D811}" name="producer_type" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{67FCCEBB-6DDF-45A8-BCEB-6CB0DC3620BC}" name="container_type" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{33672CAE-DF9C-4E5E-95C3-65F502892730}" name="container_qty" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{746F1BF1-8A1D-4807-890D-20C57B6A9E57}" name="origin" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{E2A2667F-AAD0-46D1-9AC7-050EEF762920}" name="destination" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{920927B9-F1FA-4827-887D-A0E268BEBD96}" name="container_id" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{2EC2CAEA-FB3C-4A4C-A288-E3E88A9D2E10}" name="ship_date" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{4434C7DA-1267-4C06-8242-3DE437A4BEDF}" name="delivery_date" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{D4311A9E-E2B3-4ED9-A989-6060DB766272}" name="producer" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{3EC2CE9B-5192-4531-A823-B61192F2D811}" name="producer_type" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{67FCCEBB-6DDF-45A8-BCEB-6CB0DC3620BC}" name="container_type" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{33672CAE-DF9C-4E5E-95C3-65F502892730}" name="container_qty" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{746F1BF1-8A1D-4807-890D-20C57B6A9E57}" name="origin" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{E2A2667F-AAD0-46D1-9AC7-050EEF762920}" name="destination" dataDxfId="57"/>
     <tableColumn id="10" xr3:uid="{15E56893-A5DB-4BFF-B6A9-BCA183BD2586}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{70FD1A5D-FCF6-4A1D-BBA0-AD23EECAA067}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{C68202EB-4A06-41FF-B462-9B1295D9D7CD}" name="priority" dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{04920AA8-BB38-4C51-B9D0-B839ADCC1E76}" name="status" dataDxfId="66"/>
+    <tableColumn id="12" xr3:uid="{C68202EB-4A06-41FF-B462-9B1295D9D7CD}" name="priority" dataDxfId="56"/>
+    <tableColumn id="13" xr3:uid="{04920AA8-BB38-4C51-B9D0-B839ADCC1E76}" name="status" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1951,19 +1951,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BF7484E1-5E9C-49ED-97A3-C43A408ACC38}" name="container_shipping_2020_complete" displayName="container_shipping_2020_complete" ref="A1:M25" totalsRowShown="0">
   <autoFilter ref="A1:M25" xr:uid="{BF7484E1-5E9C-49ED-97A3-C43A408ACC38}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E15B5F1B-E9E4-48D7-802A-C4F202FC60F2}" name="container_id" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{BBB46C27-D3AA-4772-B6E4-61F5C9A799F9}" name="ship_date" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{D230D201-5D0A-4889-A3FC-8F62B616BD6D}" name="delivery_date" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{F57BB7A8-5F27-4978-9C17-2D5ADFB31DB5}" name="producer" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{02CACBF7-CBCD-4E20-94CD-61DB309BA0AA}" name="producer_type" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{E8D067A1-B617-498E-96AA-8E4B4AD14E00}" name="container_type" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{B3DFFEBB-1E9C-48FD-A151-0ED750D70B27}" name="container_qty" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{5D45CC75-6E3B-4ECE-9FA0-073E24E6D4F4}" name="origin" dataDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{F0BD3D08-258D-4FA2-BF52-8464AD813DE7}" name="destination" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{E15B5F1B-E9E4-48D7-802A-C4F202FC60F2}" name="container_id" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{BBB46C27-D3AA-4772-B6E4-61F5C9A799F9}" name="ship_date" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{D230D201-5D0A-4889-A3FC-8F62B616BD6D}" name="delivery_date" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{F57BB7A8-5F27-4978-9C17-2D5ADFB31DB5}" name="producer" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{02CACBF7-CBCD-4E20-94CD-61DB309BA0AA}" name="producer_type" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{E8D067A1-B617-498E-96AA-8E4B4AD14E00}" name="container_type" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{B3DFFEBB-1E9C-48FD-A151-0ED750D70B27}" name="container_qty" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{5D45CC75-6E3B-4ECE-9FA0-073E24E6D4F4}" name="origin" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{F0BD3D08-258D-4FA2-BF52-8464AD813DE7}" name="destination" dataDxfId="46"/>
     <tableColumn id="10" xr3:uid="{6A1519EA-8E18-4753-AEF0-0FF72E13691B}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{A36006FA-2706-4E41-8ACA-AC599C323AB8}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{DAB989B3-FCE6-488C-8A70-D568B3686136}" name="priority" dataDxfId="56"/>
-    <tableColumn id="13" xr3:uid="{DE9419CA-B156-4D10-BCB4-5788AFE8F6E5}" name="status" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{DAB989B3-FCE6-488C-8A70-D568B3686136}" name="priority" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{DE9419CA-B156-4D10-BCB4-5788AFE8F6E5}" name="status" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1973,19 +1973,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3539F421-DD6B-4148-B25A-075B8D064934}" name="_2021" displayName="_2021" ref="A1:M25" totalsRowShown="0">
   <autoFilter ref="A1:M25" xr:uid="{3539F421-DD6B-4148-B25A-075B8D064934}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6BA82563-F2A3-4162-A46C-22372F4D6891}" name="container_id" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{BED2A8A4-B9F5-4D9D-812B-5660232141A3}" name="ship_date" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{87B858DD-B3AF-40BA-BD2C-E7CD55904897}" name="delivery_date" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{0E1E2A42-C43F-4969-AC59-0AB0A0277CBD}" name="producer" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{251FFB01-6133-46A5-A45C-B770C5ECBCC6}" name="producer_type" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{D72B72C5-6C12-416F-9E44-4A471CB31019}" name="container_type" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{B6C5E29A-891F-4563-B6C1-58BA782A6CAA}" name="container_qty" dataDxfId="48"/>
-    <tableColumn id="8" xr3:uid="{87E8F3CB-6FBC-477A-8104-F06B95A86706}" name="origin" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{8815CBDF-81B0-4B76-9EDC-0627594E9692}" name="destination" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{6BA82563-F2A3-4162-A46C-22372F4D6891}" name="container_id" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{BED2A8A4-B9F5-4D9D-812B-5660232141A3}" name="ship_date" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{87B858DD-B3AF-40BA-BD2C-E7CD55904897}" name="delivery_date" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{0E1E2A42-C43F-4969-AC59-0AB0A0277CBD}" name="producer" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{251FFB01-6133-46A5-A45C-B770C5ECBCC6}" name="producer_type" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{D72B72C5-6C12-416F-9E44-4A471CB31019}" name="container_type" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{B6C5E29A-891F-4563-B6C1-58BA782A6CAA}" name="container_qty" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{87E8F3CB-6FBC-477A-8104-F06B95A86706}" name="origin" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{8815CBDF-81B0-4B76-9EDC-0627594E9692}" name="destination" dataDxfId="35"/>
     <tableColumn id="10" xr3:uid="{0ADE23D1-AC2B-42BF-B222-423121681888}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{250C3991-BC28-4ED0-80A1-E71DD56ADB82}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{ABF97ABC-C63C-48E1-88DF-9D2037E0552A}" name="priority" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{E428E7BA-B18C-4271-935F-2E1DD3993C2D}" name="status" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{ABF97ABC-C63C-48E1-88DF-9D2037E0552A}" name="priority" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{E428E7BA-B18C-4271-935F-2E1DD3993C2D}" name="status" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1995,19 +1995,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E9BBC6EA-A326-47A1-A865-144217CE48E2}" name="container_shipping_2022_complete" displayName="container_shipping_2022_complete" ref="A1:M25" totalsRowShown="0">
   <autoFilter ref="A1:M25" xr:uid="{E9BBC6EA-A326-47A1-A865-144217CE48E2}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{EB306D6E-48FB-42EF-A7B5-EC5B298770B9}" name="container_id" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{4E6CEE7F-C7D3-400B-ACC5-B8F9F3D9D91A}" name="ship_date" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{52153897-EB03-40E4-91B8-A484DBBB3E8A}" name="delivery_date" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{2B4B00DB-1AB7-41F6-A9FA-0A6DD93F6D69}" name="producer" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{69E4D8E2-70C9-4432-A670-658DBADF66AD}" name="producer_type" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{A8AF4830-2C88-4022-831F-B5016BD48590}" name="container_type" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{FF25DC78-952D-44C6-9E16-79A54841E836}" name="container_qty" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{8DC84177-DAE5-48E3-B576-57408CC89BDE}" name="origin" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{9709AC77-54EF-4970-B45D-805856861C21}" name="destination" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{EB306D6E-48FB-42EF-A7B5-EC5B298770B9}" name="container_id" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{4E6CEE7F-C7D3-400B-ACC5-B8F9F3D9D91A}" name="ship_date" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{52153897-EB03-40E4-91B8-A484DBBB3E8A}" name="delivery_date" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{2B4B00DB-1AB7-41F6-A9FA-0A6DD93F6D69}" name="producer" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{69E4D8E2-70C9-4432-A670-658DBADF66AD}" name="producer_type" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{A8AF4830-2C88-4022-831F-B5016BD48590}" name="container_type" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{FF25DC78-952D-44C6-9E16-79A54841E836}" name="container_qty" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{8DC84177-DAE5-48E3-B576-57408CC89BDE}" name="origin" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{9709AC77-54EF-4970-B45D-805856861C21}" name="destination" dataDxfId="24"/>
     <tableColumn id="10" xr3:uid="{C749AE84-3A8A-4984-8731-88BC5E6D79D0}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{5B6C78CC-FB47-44D1-B8D3-8ACEBC0D5DFE}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{1701B7F6-6010-4723-B53A-49FB0F3FF90E}" name="priority" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{44DF67F1-CD36-4760-886F-A5BCE2843F7B}" name="status" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{1701B7F6-6010-4723-B53A-49FB0F3FF90E}" name="priority" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{44DF67F1-CD36-4760-886F-A5BCE2843F7B}" name="status" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2017,19 +2017,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{362BECAA-7FBF-4750-B6BE-03BE6ADC9D8D}" name="_2023" displayName="_2023" ref="A1:M25" totalsRowShown="0">
   <autoFilter ref="A1:M25" xr:uid="{362BECAA-7FBF-4750-B6BE-03BE6ADC9D8D}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{262275F6-DF59-4A26-9B18-BBC57A397D11}" name="container_id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{63DE8E51-0BFE-4ED2-8C61-E94E302AC9C1}" name="ship_date" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{909C356B-C08A-44CB-8403-226CFFD009EA}" name="delivery_date" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{7BF2B675-D81C-42EE-AE0F-0C85AF95BC0B}" name="producer" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{9514B108-72EA-4650-A902-4299D0E6DE03}" name="producer_type" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{6C63910D-EBBC-4C42-BB88-8FA61D00F2F9}" name="container_type" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{E0E646EE-62AE-4CDF-9A01-CA915DAB8A1F}" name="container_qty" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{040AFB2E-32DE-4E57-AC2E-9C484F2F5F18}" name="origin" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{5C3A41A2-2AC9-48E9-8757-A41C8A86457C}" name="destination" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{262275F6-DF59-4A26-9B18-BBC57A397D11}" name="container_id" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{63DE8E51-0BFE-4ED2-8C61-E94E302AC9C1}" name="ship_date" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{909C356B-C08A-44CB-8403-226CFFD009EA}" name="delivery_date" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7BF2B675-D81C-42EE-AE0F-0C85AF95BC0B}" name="producer" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{9514B108-72EA-4650-A902-4299D0E6DE03}" name="producer_type" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{6C63910D-EBBC-4C42-BB88-8FA61D00F2F9}" name="container_type" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{E0E646EE-62AE-4CDF-9A01-CA915DAB8A1F}" name="container_qty" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{040AFB2E-32DE-4E57-AC2E-9C484F2F5F18}" name="origin" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{5C3A41A2-2AC9-48E9-8757-A41C8A86457C}" name="destination" dataDxfId="13"/>
     <tableColumn id="10" xr3:uid="{B710A339-C9BE-4E28-B45B-97167DF25308}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{A7237D45-474E-4C6D-8235-3779FD45F272}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{FFE68D7A-1E1F-4CF4-9291-77DB2EE36023}" name="priority" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{9CABDA45-A4A7-45FE-8940-3A165B911E0F}" name="status" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{FFE68D7A-1E1F-4CF4-9291-77DB2EE36023}" name="priority" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{9CABDA45-A4A7-45FE-8940-3A165B911E0F}" name="status" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2039,19 +2039,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{BA4DF5C3-E5BF-49C8-A552-EA0322D59A25}" name="_2024" displayName="_2024" ref="A1:M25" totalsRowShown="0">
   <autoFilter ref="A1:M25" xr:uid="{BA4DF5C3-E5BF-49C8-A552-EA0322D59A25}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{3D5401C5-FF53-416C-AC4B-D41F1A2CC885}" name="container_id" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{B44FFE8B-C436-47CB-8D23-A72405D01E16}" name="ship_date" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{B268CABB-D66C-4FF9-B90B-094AF0132B66}" name="delivery_date" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{1B2E2DC6-17A5-4CB8-988B-3A0C6246E59B}" name="producer" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{964A0A45-E387-4291-94C2-D5DBD1088C4C}" name="producer_type" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{D15DD3FA-52D3-4064-A8C0-BF19F5B8108E}" name="container_type" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{378CDA3B-905D-4B70-AEA9-471064C2CAD0}" name="container_qty" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{1C34EAF7-0D3D-4A63-AB70-9D7DFED57C8A}" name="origin" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{1C6D451C-CB8A-4A6D-8794-7965B1B22C8D}" name="destination" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{3D5401C5-FF53-416C-AC4B-D41F1A2CC885}" name="container_id" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B44FFE8B-C436-47CB-8D23-A72405D01E16}" name="ship_date" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B268CABB-D66C-4FF9-B90B-094AF0132B66}" name="delivery_date" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{1B2E2DC6-17A5-4CB8-988B-3A0C6246E59B}" name="producer" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{964A0A45-E387-4291-94C2-D5DBD1088C4C}" name="producer_type" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{D15DD3FA-52D3-4064-A8C0-BF19F5B8108E}" name="container_type" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{378CDA3B-905D-4B70-AEA9-471064C2CAD0}" name="container_qty" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{1C34EAF7-0D3D-4A63-AB70-9D7DFED57C8A}" name="origin" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1C6D451C-CB8A-4A6D-8794-7965B1B22C8D}" name="destination" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{19A8E52B-8820-4EB4-9B69-022D2BC2BB05}" name="freight_index"/>
     <tableColumn id="11" xr3:uid="{8C3B9FF3-AA55-43D8-9A0F-3AB9DCEB2402}" name="base_price"/>
-    <tableColumn id="12" xr3:uid="{6C4CF0E8-F89C-49EC-AFA2-EDFCE58967B8}" name="priority" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{9019A4D0-A07A-4D05-A08C-D3BED536719C}" name="status" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{6C4CF0E8-F89C-49EC-AFA2-EDFCE58967B8}" name="priority" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{9019A4D0-A07A-4D05-A08C-D3BED536719C}" name="status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9103,7 +9103,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="J1" sqref="J1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>